<commit_message>
Added Vendors module, Products Module, WebDriver Utility
</commit_message>
<xml_diff>
--- a/vtiger-project/src/test/resources/VitigerTestCase.xlsx
+++ b/vtiger-project/src/test/resources/VitigerTestCase.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AkashDeb\eclipse-workspace_ActiTimeProject_JAN2023\vtiger-project\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="6015" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TC_4001 (Product) Prashant" sheetId="1" r:id="rId1"/>
@@ -19,6 +14,7 @@
     <sheet name="TC_6001" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A5:H22"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7miWoPtcZJ+a9fYivi9QszMQNvSmsg=="/>
@@ -2952,7 +2948,16 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2960,37 +2965,28 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3233,33 +3229,33 @@
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="160" t="s">
+      <c r="B1" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="167"/>
+    </row>
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="163"/>
+      <c r="B2" s="168"/>
       <c r="C2" s="154"/>
       <c r="D2" s="154"/>
       <c r="E2" s="154"/>
       <c r="F2" s="164"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="163" t="s">
+      <c r="B3" s="168" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="154"/>
@@ -3267,31 +3263,31 @@
       <c r="E3" s="154"/>
       <c r="F3" s="164"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="163"/>
+      <c r="B4" s="168"/>
       <c r="C4" s="154"/>
       <c r="D4" s="154"/>
       <c r="E4" s="154"/>
       <c r="F4" s="164"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="163"/>
+      <c r="B5" s="168"/>
       <c r="C5" s="154"/>
       <c r="D5" s="154"/>
       <c r="E5" s="154"/>
       <c r="F5" s="164"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="168" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="154"/>
@@ -3299,11 +3295,11 @@
       <c r="E6" s="154"/>
       <c r="F6" s="164"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="163" t="s">
+      <c r="B7" s="168" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="154"/>
@@ -3311,11 +3307,11 @@
       <c r="E7" s="154"/>
       <c r="F7" s="164"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="163" t="s">
+      <c r="B8" s="168" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="154"/>
@@ -3323,19 +3319,19 @@
       <c r="E8" s="154"/>
       <c r="F8" s="164"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="167"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="162"/>
+    </row>
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -3355,7 +3351,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>1</v>
       </c>
@@ -3369,7 +3365,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>2</v>
       </c>
@@ -3385,7 +3381,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <v>3</v>
       </c>
@@ -3399,7 +3395,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <v>4</v>
       </c>
@@ -3413,7 +3409,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="22">
         <v>5</v>
       </c>
@@ -3427,7 +3423,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="22">
         <v>6</v>
       </c>
@@ -3441,7 +3437,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="22">
         <v>7</v>
       </c>
@@ -3455,7 +3451,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="21"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="25">
         <v>8</v>
       </c>
@@ -3469,7 +3465,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="25">
         <v>9</v>
       </c>
@@ -3483,7 +3479,7 @@
       <c r="E19" s="28"/>
       <c r="F19" s="29"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="25">
         <v>10</v>
       </c>
@@ -3497,7 +3493,7 @@
       <c r="E20" s="28"/>
       <c r="F20" s="29"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="25">
         <v>11</v>
       </c>
@@ -3511,7 +3507,7 @@
       <c r="E21" s="28"/>
       <c r="F21" s="29"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="25">
         <v>12</v>
       </c>
@@ -3525,7 +3521,7 @@
       <c r="E22" s="28"/>
       <c r="F22" s="29"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="25">
         <v>13</v>
       </c>
@@ -3539,7 +3535,7 @@
       <c r="E23" s="28"/>
       <c r="F23" s="29"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="25">
         <v>14</v>
       </c>
@@ -3553,7 +3549,7 @@
       <c r="E24" s="28"/>
       <c r="F24" s="29"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="25">
         <v>15</v>
       </c>
@@ -3567,7 +3563,7 @@
       <c r="E25" s="28"/>
       <c r="F25" s="29"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="25">
         <v>16</v>
       </c>
@@ -3581,7 +3577,7 @@
       <c r="E26" s="28"/>
       <c r="F26" s="29"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="25">
         <v>17</v>
       </c>
@@ -3697,19 +3693,19 @@
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="160" t="s">
+      <c r="B35" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="161"/>
-      <c r="D35" s="161"/>
-      <c r="E35" s="161"/>
-      <c r="F35" s="162"/>
+      <c r="C35" s="166"/>
+      <c r="D35" s="166"/>
+      <c r="E35" s="166"/>
+      <c r="F35" s="167"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="163"/>
+      <c r="B36" s="168"/>
       <c r="C36" s="154"/>
       <c r="D36" s="154"/>
       <c r="E36" s="154"/>
@@ -3719,7 +3715,7 @@
       <c r="A37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="163" t="s">
+      <c r="B37" s="168" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="154"/>
@@ -3731,7 +3727,7 @@
       <c r="A38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="163" t="s">
+      <c r="B38" s="168" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="154"/>
@@ -3743,7 +3739,7 @@
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="163"/>
+      <c r="B39" s="168"/>
       <c r="C39" s="154"/>
       <c r="D39" s="154"/>
       <c r="E39" s="154"/>
@@ -3753,7 +3749,7 @@
       <c r="A40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="163" t="s">
+      <c r="B40" s="168" t="s">
         <v>68</v>
       </c>
       <c r="C40" s="154"/>
@@ -3765,7 +3761,7 @@
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="163" t="s">
+      <c r="B41" s="168" t="s">
         <v>69</v>
       </c>
       <c r="C41" s="154"/>
@@ -3777,7 +3773,7 @@
       <c r="A42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="163" t="s">
+      <c r="B42" s="168" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="154"/>
@@ -3789,13 +3785,13 @@
       <c r="A43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="165" t="s">
+      <c r="B43" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="166"/>
-      <c r="D43" s="166"/>
-      <c r="E43" s="166"/>
-      <c r="F43" s="167"/>
+      <c r="C43" s="161"/>
+      <c r="D43" s="161"/>
+      <c r="E43" s="161"/>
+      <c r="F43" s="162"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
@@ -4447,19 +4443,19 @@
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B89" s="160" t="s">
+      <c r="B89" s="170" t="s">
         <v>128</v>
       </c>
-      <c r="C89" s="161"/>
-      <c r="D89" s="161"/>
-      <c r="E89" s="161"/>
-      <c r="F89" s="162"/>
+      <c r="C89" s="166"/>
+      <c r="D89" s="166"/>
+      <c r="E89" s="166"/>
+      <c r="F89" s="167"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B90" s="168"/>
+      <c r="B90" s="163"/>
       <c r="C90" s="154"/>
       <c r="D90" s="154"/>
       <c r="E90" s="154"/>
@@ -4469,7 +4465,7 @@
       <c r="A91" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B91" s="168" t="s">
+      <c r="B91" s="163" t="s">
         <v>4</v>
       </c>
       <c r="C91" s="154"/>
@@ -4481,7 +4477,7 @@
       <c r="A92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="168" t="s">
+      <c r="B92" s="163" t="s">
         <v>129</v>
       </c>
       <c r="C92" s="154"/>
@@ -4493,7 +4489,7 @@
       <c r="A93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="168"/>
+      <c r="B93" s="163"/>
       <c r="C93" s="154"/>
       <c r="D93" s="154"/>
       <c r="E93" s="154"/>
@@ -4503,7 +4499,7 @@
       <c r="A94" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B94" s="168" t="s">
+      <c r="B94" s="163" t="s">
         <v>130</v>
       </c>
       <c r="C94" s="154"/>
@@ -4515,7 +4511,7 @@
       <c r="A95" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B95" s="168" t="s">
+      <c r="B95" s="163" t="s">
         <v>131</v>
       </c>
       <c r="C95" s="154"/>
@@ -4527,7 +4523,7 @@
       <c r="A96" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B96" s="168" t="s">
+      <c r="B96" s="163" t="s">
         <v>12</v>
       </c>
       <c r="C96" s="154"/>
@@ -4539,13 +4535,13 @@
       <c r="A97" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B97" s="169" t="s">
+      <c r="B97" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C97" s="166"/>
-      <c r="D97" s="166"/>
-      <c r="E97" s="166"/>
-      <c r="F97" s="167"/>
+      <c r="C97" s="161"/>
+      <c r="D97" s="161"/>
+      <c r="E97" s="161"/>
+      <c r="F97" s="162"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
@@ -4755,19 +4751,19 @@
       <c r="A112" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B112" s="170" t="s">
+      <c r="B112" s="165" t="s">
         <v>138</v>
       </c>
-      <c r="C112" s="161"/>
-      <c r="D112" s="161"/>
-      <c r="E112" s="161"/>
-      <c r="F112" s="162"/>
+      <c r="C112" s="166"/>
+      <c r="D112" s="166"/>
+      <c r="E112" s="166"/>
+      <c r="F112" s="167"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B113" s="168"/>
+      <c r="B113" s="163"/>
       <c r="C113" s="154"/>
       <c r="D113" s="154"/>
       <c r="E113" s="154"/>
@@ -4777,7 +4773,7 @@
       <c r="A114" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B114" s="168" t="s">
+      <c r="B114" s="163" t="s">
         <v>4</v>
       </c>
       <c r="C114" s="154"/>
@@ -4789,7 +4785,7 @@
       <c r="A115" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B115" s="168" t="s">
+      <c r="B115" s="163" t="s">
         <v>139</v>
       </c>
       <c r="C115" s="154"/>
@@ -4801,7 +4797,7 @@
       <c r="A116" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B116" s="168"/>
+      <c r="B116" s="163"/>
       <c r="C116" s="154"/>
       <c r="D116" s="154"/>
       <c r="E116" s="154"/>
@@ -4811,7 +4807,7 @@
       <c r="A117" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B117" s="168" t="s">
+      <c r="B117" s="163" t="s">
         <v>140</v>
       </c>
       <c r="C117" s="154"/>
@@ -4823,7 +4819,7 @@
       <c r="A118" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B118" s="168" t="s">
+      <c r="B118" s="163" t="s">
         <v>131</v>
       </c>
       <c r="C118" s="154"/>
@@ -4835,7 +4831,7 @@
       <c r="A119" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="168" t="s">
+      <c r="B119" s="163" t="s">
         <v>12</v>
       </c>
       <c r="C119" s="154"/>
@@ -4847,13 +4843,13 @@
       <c r="A120" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B120" s="169" t="s">
+      <c r="B120" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="166"/>
-      <c r="D120" s="166"/>
-      <c r="E120" s="166"/>
-      <c r="F120" s="167"/>
+      <c r="C120" s="161"/>
+      <c r="D120" s="161"/>
+      <c r="E120" s="161"/>
+      <c r="F120" s="162"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
@@ -6157,6 +6153,65 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
     <mergeCell ref="B159:F159"/>
     <mergeCell ref="B160:F160"/>
     <mergeCell ref="B161:F161"/>
@@ -6166,65 +6221,6 @@
     <mergeCell ref="B140:F140"/>
     <mergeCell ref="B142:F142"/>
     <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
@@ -6249,7 +6245,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -6295,7 +6291,7 @@
       <c r="A2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="172" t="s">
         <v>221</v>
       </c>
       <c r="C2" s="154"/>
@@ -6323,7 +6319,7 @@
       <c r="A3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="172" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="154"/>
@@ -6351,7 +6347,7 @@
       <c r="A4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="172" t="s">
         <v>222</v>
       </c>
       <c r="C4" s="154"/>
@@ -6379,7 +6375,7 @@
       <c r="A5" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="171"/>
+      <c r="B5" s="172"/>
       <c r="C5" s="154"/>
       <c r="D5" s="154"/>
       <c r="E5" s="154"/>
@@ -6405,7 +6401,7 @@
       <c r="A6" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="172" t="s">
         <v>223</v>
       </c>
       <c r="C6" s="154"/>
@@ -6433,7 +6429,7 @@
       <c r="A7" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="171" t="s">
+      <c r="B7" s="172" t="s">
         <v>224</v>
       </c>
       <c r="C7" s="154"/>
@@ -6461,7 +6457,7 @@
       <c r="A8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="171" t="s">
+      <c r="B8" s="172" t="s">
         <v>225</v>
       </c>
       <c r="C8" s="154"/>
@@ -7199,7 +7195,7 @@
       <c r="A32" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="171" t="s">
+      <c r="B32" s="172" t="s">
         <v>259</v>
       </c>
       <c r="C32" s="154"/>
@@ -7228,7 +7224,7 @@
       <c r="A33" s="81" t="s">
         <v>260</v>
       </c>
-      <c r="B33" s="171" t="s">
+      <c r="B33" s="172" t="s">
         <v>261</v>
       </c>
       <c r="C33" s="154"/>
@@ -7257,7 +7253,7 @@
       <c r="A34" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="171" t="s">
+      <c r="B34" s="172" t="s">
         <v>262</v>
       </c>
       <c r="C34" s="154"/>
@@ -7286,7 +7282,7 @@
       <c r="A35" s="81" t="s">
         <v>263</v>
       </c>
-      <c r="B35" s="171"/>
+      <c r="B35" s="172"/>
       <c r="C35" s="154"/>
       <c r="D35" s="154"/>
       <c r="E35" s="154"/>
@@ -7313,7 +7309,7 @@
       <c r="A36" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="B36" s="171" t="s">
+      <c r="B36" s="172" t="s">
         <v>264</v>
       </c>
       <c r="C36" s="154"/>
@@ -7342,7 +7338,7 @@
       <c r="A37" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="171" t="s">
+      <c r="B37" s="172" t="s">
         <v>224</v>
       </c>
       <c r="C37" s="154"/>
@@ -7371,7 +7367,7 @@
       <c r="A38" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="171" t="s">
+      <c r="B38" s="172" t="s">
         <v>225</v>
       </c>
       <c r="C38" s="154"/>
@@ -8240,7 +8236,7 @@
       <c r="A66" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="B66" s="172" t="s">
+      <c r="B66" s="171" t="s">
         <v>289</v>
       </c>
       <c r="C66" s="157"/>
@@ -8272,7 +8268,7 @@
       <c r="A67" s="89" t="s">
         <v>260</v>
       </c>
-      <c r="B67" s="172" t="s">
+      <c r="B67" s="171" t="s">
         <v>290</v>
       </c>
       <c r="C67" s="157"/>
@@ -8304,7 +8300,7 @@
       <c r="A68" s="89" t="s">
         <v>146</v>
       </c>
-      <c r="B68" s="172" t="s">
+      <c r="B68" s="171" t="s">
         <v>262</v>
       </c>
       <c r="C68" s="157"/>
@@ -8366,7 +8362,7 @@
       <c r="A70" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="B70" s="172" t="s">
+      <c r="B70" s="171" t="s">
         <v>264</v>
       </c>
       <c r="C70" s="157"/>
@@ -8398,7 +8394,7 @@
       <c r="A71" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B71" s="172" t="s">
+      <c r="B71" s="171" t="s">
         <v>224</v>
       </c>
       <c r="C71" s="157"/>
@@ -8430,7 +8426,7 @@
       <c r="A72" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B72" s="172" t="s">
+      <c r="B72" s="171" t="s">
         <v>225</v>
       </c>
       <c r="C72" s="157"/>
@@ -9855,6 +9851,16 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
     <mergeCell ref="B69:F69"/>
     <mergeCell ref="B70:F70"/>
     <mergeCell ref="B71:F71"/>
@@ -9866,16 +9872,6 @@
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
@@ -9895,7 +9891,7 @@
   </sheetPr>
   <dimension ref="A1:W1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9938,7 +9934,7 @@
       <c r="A2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="171"/>
+      <c r="B2" s="172"/>
       <c r="C2" s="154"/>
       <c r="D2" s="154"/>
       <c r="E2" s="154"/>
@@ -9964,7 +9960,7 @@
       <c r="A3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="172" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="154"/>
@@ -9992,7 +9988,7 @@
       <c r="A4" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="171"/>
+      <c r="B4" s="172"/>
       <c r="C4" s="154"/>
       <c r="D4" s="154"/>
       <c r="E4" s="154"/>
@@ -10018,7 +10014,7 @@
       <c r="A5" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="171"/>
+      <c r="B5" s="172"/>
       <c r="C5" s="154"/>
       <c r="D5" s="154"/>
       <c r="E5" s="154"/>
@@ -10044,7 +10040,7 @@
       <c r="A6" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="172" t="s">
         <v>303</v>
       </c>
       <c r="C6" s="154"/>
@@ -10072,7 +10068,7 @@
       <c r="A7" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="171" t="s">
+      <c r="B7" s="172" t="s">
         <v>304</v>
       </c>
       <c r="C7" s="154"/>
@@ -10128,7 +10124,7 @@
       <c r="A9" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="171"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="154"/>
       <c r="D9" s="154"/>
       <c r="E9" s="154"/>
@@ -10548,7 +10544,7 @@
       <c r="A23" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="173" t="s">
+      <c r="B23" s="176" t="s">
         <v>314</v>
       </c>
       <c r="C23" s="154"/>
@@ -10577,7 +10573,7 @@
       <c r="A24" s="81" t="s">
         <v>260</v>
       </c>
-      <c r="B24" s="173" t="s">
+      <c r="B24" s="176" t="s">
         <v>261</v>
       </c>
       <c r="C24" s="154"/>
@@ -10606,7 +10602,7 @@
       <c r="A25" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="171"/>
+      <c r="B25" s="172"/>
       <c r="C25" s="154"/>
       <c r="D25" s="154"/>
       <c r="E25" s="154"/>
@@ -10633,7 +10629,7 @@
       <c r="A26" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="171"/>
+      <c r="B26" s="172"/>
       <c r="C26" s="154"/>
       <c r="D26" s="154"/>
       <c r="E26" s="154"/>
@@ -10660,7 +10656,7 @@
       <c r="A27" s="81" t="s">
         <v>263</v>
       </c>
-      <c r="B27" s="171"/>
+      <c r="B27" s="172"/>
       <c r="C27" s="154"/>
       <c r="D27" s="154"/>
       <c r="E27" s="154"/>
@@ -10687,7 +10683,7 @@
       <c r="A28" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="B28" s="171"/>
+      <c r="B28" s="172"/>
       <c r="C28" s="154"/>
       <c r="D28" s="154"/>
       <c r="E28" s="154"/>
@@ -10764,7 +10760,7 @@
       <c r="A31" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="171"/>
+      <c r="B31" s="172"/>
       <c r="C31" s="154"/>
       <c r="D31" s="154"/>
       <c r="E31" s="154"/>
@@ -10791,7 +10787,7 @@
       <c r="A32" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="171"/>
+      <c r="B32" s="172"/>
       <c r="C32" s="154"/>
       <c r="D32" s="154"/>
       <c r="E32" s="154"/>
@@ -11105,7 +11101,7 @@
       <c r="A44" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="174"/>
+      <c r="B44" s="173"/>
       <c r="C44" s="155"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
@@ -11159,7 +11155,7 @@
       <c r="A46" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="176"/>
+      <c r="B46" s="174"/>
       <c r="C46" s="155"/>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
@@ -11240,7 +11236,7 @@
       <c r="A49" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="B49" s="176"/>
+      <c r="B49" s="174"/>
       <c r="C49" s="155"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
@@ -11267,7 +11263,7 @@
       <c r="A50" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="176"/>
+      <c r="B50" s="174"/>
       <c r="C50" s="155"/>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
@@ -11294,7 +11290,7 @@
       <c r="A51" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B51" s="176"/>
+      <c r="B51" s="174"/>
       <c r="C51" s="155"/>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
@@ -11533,7 +11529,7 @@
       <c r="A60" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="174" t="s">
+      <c r="B60" s="173" t="s">
         <v>315</v>
       </c>
       <c r="C60" s="154"/>
@@ -11562,7 +11558,7 @@
       <c r="A61" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="174"/>
+      <c r="B61" s="173"/>
       <c r="C61" s="154"/>
       <c r="D61" s="154"/>
       <c r="E61" s="154"/>
@@ -11589,7 +11585,7 @@
       <c r="A62" s="71" t="s">
         <v>316</v>
       </c>
-      <c r="B62" s="174"/>
+      <c r="B62" s="173"/>
       <c r="C62" s="154"/>
       <c r="D62" s="154"/>
       <c r="E62" s="154"/>
@@ -11616,7 +11612,7 @@
       <c r="A63" s="71" t="s">
         <v>148</v>
       </c>
-      <c r="B63" s="174"/>
+      <c r="B63" s="173"/>
       <c r="C63" s="154"/>
       <c r="D63" s="154"/>
       <c r="E63" s="154"/>
@@ -11643,7 +11639,7 @@
       <c r="A64" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="174"/>
+      <c r="B64" s="173"/>
       <c r="C64" s="154"/>
       <c r="D64" s="154"/>
       <c r="E64" s="154"/>
@@ -11670,7 +11666,7 @@
       <c r="A65" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="174"/>
+      <c r="B65" s="173"/>
       <c r="C65" s="154"/>
       <c r="D65" s="154"/>
       <c r="E65" s="154"/>
@@ -11697,7 +11693,7 @@
       <c r="A66" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B66" s="174"/>
+      <c r="B66" s="173"/>
       <c r="C66" s="154"/>
       <c r="D66" s="154"/>
       <c r="E66" s="154"/>
@@ -11724,7 +11720,7 @@
       <c r="A67" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B67" s="174"/>
+      <c r="B67" s="173"/>
       <c r="C67" s="154"/>
       <c r="D67" s="154"/>
       <c r="E67" s="154"/>
@@ -12013,7 +12009,7 @@
       <c r="A78" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="171"/>
+      <c r="B78" s="172"/>
       <c r="C78" s="154"/>
       <c r="D78" s="154"/>
       <c r="E78" s="154"/>
@@ -12040,7 +12036,7 @@
       <c r="A79" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B79" s="171"/>
+      <c r="B79" s="172"/>
       <c r="C79" s="154"/>
       <c r="D79" s="154"/>
       <c r="E79" s="154"/>
@@ -12067,7 +12063,7 @@
       <c r="A80" s="71" t="s">
         <v>318</v>
       </c>
-      <c r="B80" s="171"/>
+      <c r="B80" s="172"/>
       <c r="C80" s="154"/>
       <c r="D80" s="154"/>
       <c r="E80" s="154"/>
@@ -12094,7 +12090,7 @@
       <c r="A81" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="171"/>
+      <c r="B81" s="172"/>
       <c r="C81" s="154"/>
       <c r="D81" s="154"/>
       <c r="E81" s="154"/>
@@ -12121,7 +12117,7 @@
       <c r="A82" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="171"/>
+      <c r="B82" s="172"/>
       <c r="C82" s="154"/>
       <c r="D82" s="154"/>
       <c r="E82" s="154"/>
@@ -12148,7 +12144,7 @@
       <c r="A83" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="171"/>
+      <c r="B83" s="172"/>
       <c r="C83" s="154"/>
       <c r="D83" s="154"/>
       <c r="E83" s="154"/>
@@ -12175,7 +12171,7 @@
       <c r="A84" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B84" s="171"/>
+      <c r="B84" s="172"/>
       <c r="C84" s="154"/>
       <c r="D84" s="154"/>
       <c r="E84" s="154"/>
@@ -12514,7 +12510,7 @@
       <c r="A97" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B97" s="171"/>
+      <c r="B97" s="172"/>
       <c r="C97" s="154"/>
       <c r="D97" s="154"/>
       <c r="E97" s="154"/>
@@ -12541,7 +12537,7 @@
       <c r="A98" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B98" s="171"/>
+      <c r="B98" s="172"/>
       <c r="C98" s="154"/>
       <c r="D98" s="154"/>
       <c r="E98" s="154"/>
@@ -12568,7 +12564,7 @@
       <c r="A99" s="71" t="s">
         <v>319</v>
       </c>
-      <c r="B99" s="171"/>
+      <c r="B99" s="172"/>
       <c r="C99" s="154"/>
       <c r="D99" s="154"/>
       <c r="E99" s="154"/>
@@ -12595,7 +12591,7 @@
       <c r="A100" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="171"/>
+      <c r="B100" s="172"/>
       <c r="C100" s="154"/>
       <c r="D100" s="154"/>
       <c r="E100" s="154"/>
@@ -12622,7 +12618,7 @@
       <c r="A101" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="171"/>
+      <c r="B101" s="172"/>
       <c r="C101" s="154"/>
       <c r="D101" s="154"/>
       <c r="E101" s="154"/>
@@ -12649,7 +12645,7 @@
       <c r="A102" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="171"/>
+      <c r="B102" s="172"/>
       <c r="C102" s="154"/>
       <c r="D102" s="154"/>
       <c r="E102" s="154"/>
@@ -12676,7 +12672,7 @@
       <c r="A103" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B103" s="171"/>
+      <c r="B103" s="172"/>
       <c r="C103" s="154"/>
       <c r="D103" s="154"/>
       <c r="E103" s="154"/>
@@ -17984,6 +17980,41 @@
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
     <mergeCell ref="B101:F101"/>
     <mergeCell ref="B102:F102"/>
     <mergeCell ref="B103:F103"/>
@@ -17994,41 +18025,6 @@
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B99:F99"/>
     <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
@@ -18394,7 +18390,7 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Added Product Module, Addded to Creating ProductPage, Added ProductInformation page
</commit_message>
<xml_diff>
--- a/vtiger-project/src/test/resources/VitigerTestCase.xlsx
+++ b/vtiger-project/src/test/resources/VitigerTestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="6015" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12885" windowHeight="3630"/>
   </bookViews>
   <sheets>
     <sheet name="TC_4001 (Product) Prashant" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="TC_6001" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A5:H22"/>
+  <oleSize ref="A1:C12"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7miWoPtcZJ+a9fYivi9QszMQNvSmsg=="/>
@@ -2948,7 +2948,16 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2956,37 +2965,28 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3217,7 +3217,9 @@
   </sheetPr>
   <dimension ref="A1:F222"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3233,19 +3235,19 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="170" t="s">
+      <c r="B1" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="167"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="168"/>
+      <c r="B2" s="163"/>
       <c r="C2" s="154"/>
       <c r="D2" s="154"/>
       <c r="E2" s="154"/>
@@ -3255,7 +3257,7 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="163" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="154"/>
@@ -3267,7 +3269,7 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="168"/>
+      <c r="B4" s="163"/>
       <c r="C4" s="154"/>
       <c r="D4" s="154"/>
       <c r="E4" s="154"/>
@@ -3277,7 +3279,7 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="168"/>
+      <c r="B5" s="163"/>
       <c r="C5" s="154"/>
       <c r="D5" s="154"/>
       <c r="E5" s="154"/>
@@ -3287,7 +3289,7 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="168" t="s">
+      <c r="B6" s="163" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="154"/>
@@ -3299,7 +3301,7 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="168" t="s">
+      <c r="B7" s="163" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="154"/>
@@ -3311,7 +3313,7 @@
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="168" t="s">
+      <c r="B8" s="163" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="154"/>
@@ -3323,13 +3325,13 @@
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="169" t="s">
+      <c r="B9" s="165" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="161"/>
-      <c r="D9" s="161"/>
-      <c r="E9" s="161"/>
-      <c r="F9" s="162"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="167"/>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -3591,7 +3593,7 @@
       <c r="E27" s="28"/>
       <c r="F27" s="29"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="25">
         <v>18</v>
       </c>
@@ -3605,7 +3607,7 @@
       <c r="E28" s="28"/>
       <c r="F28" s="29"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="25">
         <v>19</v>
       </c>
@@ -3619,7 +3621,7 @@
       <c r="E29" s="28"/>
       <c r="F29" s="29"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="25">
         <v>20</v>
       </c>
@@ -3633,7 +3635,7 @@
       <c r="E30" s="28"/>
       <c r="F30" s="29"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="25">
         <v>21</v>
       </c>
@@ -3647,7 +3649,7 @@
       <c r="E31" s="28"/>
       <c r="F31" s="29"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="25">
         <v>22</v>
       </c>
@@ -3661,7 +3663,7 @@
       <c r="E32" s="28"/>
       <c r="F32" s="29"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="25">
         <v>23</v>
       </c>
@@ -3675,7 +3677,7 @@
       <c r="E33" s="28"/>
       <c r="F33" s="29"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="25">
         <v>24</v>
       </c>
@@ -3689,33 +3691,33 @@
       <c r="E34" s="28"/>
       <c r="F34" s="29"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="170" t="s">
+      <c r="B35" s="160" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="166"/>
-      <c r="D35" s="166"/>
-      <c r="E35" s="166"/>
-      <c r="F35" s="167"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="161"/>
+      <c r="D35" s="161"/>
+      <c r="E35" s="161"/>
+      <c r="F35" s="162"/>
+    </row>
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="168"/>
+      <c r="B36" s="163"/>
       <c r="C36" s="154"/>
       <c r="D36" s="154"/>
       <c r="E36" s="154"/>
       <c r="F36" s="164"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="168" t="s">
+      <c r="B37" s="163" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="154"/>
@@ -3723,11 +3725,11 @@
       <c r="E37" s="154"/>
       <c r="F37" s="164"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="168" t="s">
+      <c r="B38" s="163" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="154"/>
@@ -3735,21 +3737,21 @@
       <c r="E38" s="154"/>
       <c r="F38" s="164"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="168"/>
+      <c r="B39" s="163"/>
       <c r="C39" s="154"/>
       <c r="D39" s="154"/>
       <c r="E39" s="154"/>
       <c r="F39" s="164"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="168" t="s">
+      <c r="B40" s="163" t="s">
         <v>68</v>
       </c>
       <c r="C40" s="154"/>
@@ -3757,11 +3759,11 @@
       <c r="E40" s="154"/>
       <c r="F40" s="164"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="168" t="s">
+      <c r="B41" s="163" t="s">
         <v>69</v>
       </c>
       <c r="C41" s="154"/>
@@ -3769,11 +3771,11 @@
       <c r="E41" s="154"/>
       <c r="F41" s="164"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="168" t="s">
+      <c r="B42" s="163" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="154"/>
@@ -3781,19 +3783,19 @@
       <c r="E42" s="154"/>
       <c r="F42" s="164"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="169" t="s">
+      <c r="B43" s="165" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="161"/>
-      <c r="D43" s="161"/>
-      <c r="E43" s="161"/>
-      <c r="F43" s="162"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="166"/>
+      <c r="D43" s="166"/>
+      <c r="E43" s="166"/>
+      <c r="F43" s="167"/>
+    </row>
+    <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>15</v>
       </c>
@@ -3813,7 +3815,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <v>1</v>
       </c>
@@ -3827,7 +3829,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="15"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="16">
         <v>2</v>
       </c>
@@ -3843,7 +3845,7 @@
       <c r="E46" s="20"/>
       <c r="F46" s="21"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="22">
         <v>3</v>
       </c>
@@ -3857,7 +3859,7 @@
       <c r="E47" s="20"/>
       <c r="F47" s="21"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="22">
         <v>4</v>
       </c>
@@ -3871,7 +3873,7 @@
       <c r="E48" s="20"/>
       <c r="F48" s="21"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="22">
         <v>5</v>
       </c>
@@ -3885,7 +3887,7 @@
       <c r="E49" s="20"/>
       <c r="F49" s="21"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="22">
         <v>6</v>
       </c>
@@ -3899,7 +3901,7 @@
       <c r="E50" s="20"/>
       <c r="F50" s="21"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="22">
         <v>7</v>
       </c>
@@ -3913,7 +3915,7 @@
       <c r="E51" s="20"/>
       <c r="F51" s="21"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="25">
         <v>8</v>
       </c>
@@ -3927,7 +3929,7 @@
       <c r="E52" s="20"/>
       <c r="F52" s="21"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="25">
         <v>9</v>
       </c>
@@ -3941,7 +3943,7 @@
       <c r="E53" s="28"/>
       <c r="F53" s="29"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="30">
         <v>10</v>
       </c>
@@ -3955,7 +3957,7 @@
       <c r="E54" s="33"/>
       <c r="F54" s="34"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="25">
         <v>11</v>
       </c>
@@ -3969,7 +3971,7 @@
       <c r="E55" s="28"/>
       <c r="F55" s="29"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="22">
         <v>12</v>
       </c>
@@ -3983,7 +3985,7 @@
       <c r="E56" s="28"/>
       <c r="F56" s="29"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="25">
         <v>13</v>
       </c>
@@ -3997,7 +3999,7 @@
       <c r="E57" s="28"/>
       <c r="F57" s="29"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="25">
         <v>14</v>
       </c>
@@ -4011,7 +4013,7 @@
       <c r="E58" s="28"/>
       <c r="F58" s="29"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="30">
         <v>15</v>
       </c>
@@ -4025,7 +4027,7 @@
       <c r="E59" s="28"/>
       <c r="F59" s="29"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="25">
         <v>16</v>
       </c>
@@ -4039,7 +4041,7 @@
       <c r="E60" s="28"/>
       <c r="F60" s="29"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="22">
         <v>17</v>
       </c>
@@ -4055,7 +4057,7 @@
       <c r="E61" s="28"/>
       <c r="F61" s="29"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="25">
         <v>18</v>
       </c>
@@ -4069,7 +4071,7 @@
       <c r="E62" s="28"/>
       <c r="F62" s="29"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="25">
         <v>19</v>
       </c>
@@ -4083,7 +4085,7 @@
       <c r="E63" s="28"/>
       <c r="F63" s="29"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="30">
         <v>20</v>
       </c>
@@ -4097,7 +4099,7 @@
       <c r="E64" s="28"/>
       <c r="F64" s="29"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="25">
         <v>21</v>
       </c>
@@ -4111,7 +4113,7 @@
       <c r="E65" s="28"/>
       <c r="F65" s="29"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="22">
         <v>22</v>
       </c>
@@ -4125,7 +4127,7 @@
       <c r="E66" s="28"/>
       <c r="F66" s="29"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="25">
         <v>23</v>
       </c>
@@ -4139,7 +4141,7 @@
       <c r="E67" s="28"/>
       <c r="F67" s="29"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="25">
         <v>24</v>
       </c>
@@ -4153,7 +4155,7 @@
       <c r="E68" s="28"/>
       <c r="F68" s="29"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="30">
         <v>25</v>
       </c>
@@ -4167,7 +4169,7 @@
       <c r="E69" s="28"/>
       <c r="F69" s="29"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="25">
         <v>26</v>
       </c>
@@ -4183,7 +4185,7 @@
       <c r="E70" s="28"/>
       <c r="F70" s="29"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="22">
         <v>27</v>
       </c>
@@ -4197,7 +4199,7 @@
       <c r="E71" s="28"/>
       <c r="F71" s="29"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="25">
         <v>28</v>
       </c>
@@ -4213,7 +4215,7 @@
       <c r="E72" s="28"/>
       <c r="F72" s="29"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="25">
         <v>29</v>
       </c>
@@ -4227,7 +4229,7 @@
       <c r="E73" s="28"/>
       <c r="F73" s="29"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="30">
         <v>30</v>
       </c>
@@ -4243,7 +4245,7 @@
       <c r="E74" s="28"/>
       <c r="F74" s="29"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="25">
         <v>31</v>
       </c>
@@ -4257,7 +4259,7 @@
       <c r="E75" s="28"/>
       <c r="F75" s="29"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="22">
         <v>32</v>
       </c>
@@ -4271,7 +4273,7 @@
       <c r="E76" s="28"/>
       <c r="F76" s="29"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="25">
         <v>33</v>
       </c>
@@ -4285,7 +4287,7 @@
       <c r="E77" s="28"/>
       <c r="F77" s="29"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="25">
         <v>34</v>
       </c>
@@ -4299,7 +4301,7 @@
       <c r="E78" s="28"/>
       <c r="F78" s="29"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="30">
         <v>35</v>
       </c>
@@ -4313,7 +4315,7 @@
       <c r="E79" s="28"/>
       <c r="F79" s="29"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="25">
         <v>36</v>
       </c>
@@ -4327,7 +4329,7 @@
       <c r="E80" s="28"/>
       <c r="F80" s="29"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="22">
         <v>37</v>
       </c>
@@ -4341,7 +4343,7 @@
       <c r="E81" s="28"/>
       <c r="F81" s="29"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="25">
         <v>38</v>
       </c>
@@ -4357,7 +4359,7 @@
       <c r="E82" s="28"/>
       <c r="F82" s="29"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="25">
         <v>39</v>
       </c>
@@ -4371,7 +4373,7 @@
       <c r="E83" s="28"/>
       <c r="F83" s="29"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="30">
         <v>40</v>
       </c>
@@ -4385,7 +4387,7 @@
       <c r="E84" s="28"/>
       <c r="F84" s="29"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="25">
         <v>41</v>
       </c>
@@ -4399,7 +4401,7 @@
       <c r="E85" s="28"/>
       <c r="F85" s="29"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="22">
         <v>42</v>
       </c>
@@ -4411,7 +4413,7 @@
       <c r="E86" s="28"/>
       <c r="F86" s="29"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="25">
         <v>43</v>
       </c>
@@ -4425,7 +4427,7 @@
       <c r="E87" s="28"/>
       <c r="F87" s="29"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="25">
         <v>44</v>
       </c>
@@ -4439,33 +4441,33 @@
       <c r="E88" s="28"/>
       <c r="F88" s="29"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B89" s="170" t="s">
+      <c r="B89" s="160" t="s">
         <v>128</v>
       </c>
-      <c r="C89" s="166"/>
-      <c r="D89" s="166"/>
-      <c r="E89" s="166"/>
-      <c r="F89" s="167"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C89" s="161"/>
+      <c r="D89" s="161"/>
+      <c r="E89" s="161"/>
+      <c r="F89" s="162"/>
+    </row>
+    <row r="90" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B90" s="163"/>
+      <c r="B90" s="168"/>
       <c r="C90" s="154"/>
       <c r="D90" s="154"/>
       <c r="E90" s="154"/>
       <c r="F90" s="164"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B91" s="163" t="s">
+      <c r="B91" s="168" t="s">
         <v>4</v>
       </c>
       <c r="C91" s="154"/>
@@ -4473,11 +4475,11 @@
       <c r="E91" s="154"/>
       <c r="F91" s="164"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="163" t="s">
+      <c r="B92" s="168" t="s">
         <v>129</v>
       </c>
       <c r="C92" s="154"/>
@@ -4485,21 +4487,21 @@
       <c r="E92" s="154"/>
       <c r="F92" s="164"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="163"/>
+      <c r="B93" s="168"/>
       <c r="C93" s="154"/>
       <c r="D93" s="154"/>
       <c r="E93" s="154"/>
       <c r="F93" s="164"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B94" s="163" t="s">
+      <c r="B94" s="168" t="s">
         <v>130</v>
       </c>
       <c r="C94" s="154"/>
@@ -4507,11 +4509,11 @@
       <c r="E94" s="154"/>
       <c r="F94" s="164"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B95" s="163" t="s">
+      <c r="B95" s="168" t="s">
         <v>131</v>
       </c>
       <c r="C95" s="154"/>
@@ -4519,11 +4521,11 @@
       <c r="E95" s="154"/>
       <c r="F95" s="164"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B96" s="163" t="s">
+      <c r="B96" s="168" t="s">
         <v>12</v>
       </c>
       <c r="C96" s="154"/>
@@ -4531,19 +4533,19 @@
       <c r="E96" s="154"/>
       <c r="F96" s="164"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B97" s="160" t="s">
+      <c r="B97" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="C97" s="161"/>
-      <c r="D97" s="161"/>
-      <c r="E97" s="161"/>
-      <c r="F97" s="162"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C97" s="166"/>
+      <c r="D97" s="166"/>
+      <c r="E97" s="166"/>
+      <c r="F97" s="167"/>
+    </row>
+    <row r="98" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>15</v>
       </c>
@@ -4563,7 +4565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="16">
         <v>1</v>
       </c>
@@ -4577,7 +4579,7 @@
       <c r="E99" s="20"/>
       <c r="F99" s="21"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="16">
         <v>2</v>
       </c>
@@ -4593,7 +4595,7 @@
       <c r="E100" s="20"/>
       <c r="F100" s="21"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="22">
         <v>3</v>
       </c>
@@ -4607,7 +4609,7 @@
       <c r="E101" s="20"/>
       <c r="F101" s="21"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="22">
         <v>4</v>
       </c>
@@ -4621,7 +4623,7 @@
       <c r="E102" s="20"/>
       <c r="F102" s="21"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="22">
         <v>5</v>
       </c>
@@ -4635,7 +4637,7 @@
       <c r="E103" s="20"/>
       <c r="F103" s="21"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="22">
         <v>6</v>
       </c>
@@ -4649,7 +4651,7 @@
       <c r="E104" s="20"/>
       <c r="F104" s="21"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="22">
         <v>7</v>
       </c>
@@ -4665,7 +4667,7 @@
       <c r="E105" s="20"/>
       <c r="F105" s="21"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="25">
         <v>8</v>
       </c>
@@ -4679,7 +4681,7 @@
       <c r="E106" s="20"/>
       <c r="F106" s="21"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="25">
         <v>9</v>
       </c>
@@ -4693,7 +4695,7 @@
       <c r="E107" s="28"/>
       <c r="F107" s="29"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="30">
         <v>10</v>
       </c>
@@ -4707,7 +4709,7 @@
       <c r="E108" s="33"/>
       <c r="F108" s="34"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="25">
         <v>11</v>
       </c>
@@ -4719,7 +4721,7 @@
       <c r="E109" s="28"/>
       <c r="F109" s="29"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="25">
         <v>12</v>
       </c>
@@ -4733,7 +4735,7 @@
       <c r="E110" s="28"/>
       <c r="F110" s="29"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="25">
         <v>13</v>
       </c>
@@ -4747,33 +4749,33 @@
       <c r="E111" s="28"/>
       <c r="F111" s="29"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B112" s="165" t="s">
+      <c r="B112" s="170" t="s">
         <v>138</v>
       </c>
-      <c r="C112" s="166"/>
-      <c r="D112" s="166"/>
-      <c r="E112" s="166"/>
-      <c r="F112" s="167"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C112" s="161"/>
+      <c r="D112" s="161"/>
+      <c r="E112" s="161"/>
+      <c r="F112" s="162"/>
+    </row>
+    <row r="113" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B113" s="163"/>
+      <c r="B113" s="168"/>
       <c r="C113" s="154"/>
       <c r="D113" s="154"/>
       <c r="E113" s="154"/>
       <c r="F113" s="164"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B114" s="163" t="s">
+      <c r="B114" s="168" t="s">
         <v>4</v>
       </c>
       <c r="C114" s="154"/>
@@ -4781,11 +4783,11 @@
       <c r="E114" s="154"/>
       <c r="F114" s="164"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B115" s="163" t="s">
+      <c r="B115" s="168" t="s">
         <v>139</v>
       </c>
       <c r="C115" s="154"/>
@@ -4793,21 +4795,21 @@
       <c r="E115" s="154"/>
       <c r="F115" s="164"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B116" s="163"/>
+      <c r="B116" s="168"/>
       <c r="C116" s="154"/>
       <c r="D116" s="154"/>
       <c r="E116" s="154"/>
       <c r="F116" s="164"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B117" s="163" t="s">
+      <c r="B117" s="168" t="s">
         <v>140</v>
       </c>
       <c r="C117" s="154"/>
@@ -4815,11 +4817,11 @@
       <c r="E117" s="154"/>
       <c r="F117" s="164"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B118" s="163" t="s">
+      <c r="B118" s="168" t="s">
         <v>131</v>
       </c>
       <c r="C118" s="154"/>
@@ -4827,11 +4829,11 @@
       <c r="E118" s="154"/>
       <c r="F118" s="164"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="163" t="s">
+      <c r="B119" s="168" t="s">
         <v>12</v>
       </c>
       <c r="C119" s="154"/>
@@ -4839,19 +4841,19 @@
       <c r="E119" s="154"/>
       <c r="F119" s="164"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B120" s="160" t="s">
+      <c r="B120" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="161"/>
-      <c r="D120" s="161"/>
-      <c r="E120" s="161"/>
-      <c r="F120" s="162"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C120" s="166"/>
+      <c r="D120" s="166"/>
+      <c r="E120" s="166"/>
+      <c r="F120" s="167"/>
+    </row>
+    <row r="121" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>15</v>
       </c>
@@ -4871,7 +4873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="36">
         <v>1</v>
       </c>
@@ -4885,7 +4887,7 @@
       <c r="E122" s="40"/>
       <c r="F122" s="41"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="16">
         <v>2</v>
       </c>
@@ -4901,7 +4903,7 @@
       <c r="E123" s="20"/>
       <c r="F123" s="21"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="22">
         <v>3</v>
       </c>
@@ -4915,7 +4917,7 @@
       <c r="E124" s="20"/>
       <c r="F124" s="21"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="22">
         <v>4</v>
       </c>
@@ -4929,7 +4931,7 @@
       <c r="E125" s="20"/>
       <c r="F125" s="21"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="22">
         <v>5</v>
       </c>
@@ -4943,7 +4945,7 @@
       <c r="E126" s="20"/>
       <c r="F126" s="21"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="22">
         <v>6</v>
       </c>
@@ -4957,7 +4959,7 @@
       <c r="E127" s="20"/>
       <c r="F127" s="21"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="22">
         <v>7</v>
       </c>
@@ -4973,7 +4975,7 @@
       <c r="E128" s="20"/>
       <c r="F128" s="21"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="25">
         <v>8</v>
       </c>
@@ -4987,7 +4989,7 @@
       <c r="E129" s="20"/>
       <c r="F129" s="21"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="25">
         <v>9</v>
       </c>
@@ -5001,7 +5003,7 @@
       <c r="E130" s="28"/>
       <c r="F130" s="29"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="30">
         <v>10</v>
       </c>
@@ -5015,7 +5017,7 @@
       <c r="E131" s="33"/>
       <c r="F131" s="34"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="42">
         <v>11</v>
       </c>
@@ -5029,7 +5031,7 @@
       <c r="E132" s="44"/>
       <c r="F132" s="46"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="47" t="s">
         <v>2</v>
       </c>
@@ -5041,7 +5043,7 @@
       <c r="E134" s="154"/>
       <c r="F134" s="155"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="48" t="s">
         <v>3</v>
       </c>
@@ -5053,7 +5055,7 @@
       <c r="E135" s="154"/>
       <c r="F135" s="155"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="48" t="s">
         <v>146</v>
       </c>
@@ -5065,7 +5067,7 @@
       <c r="E136" s="154"/>
       <c r="F136" s="155"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="48" t="s">
         <v>148</v>
       </c>
@@ -5075,7 +5077,7 @@
       <c r="E137" s="157"/>
       <c r="F137" s="158"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="48" t="s">
         <v>6</v>
       </c>
@@ -5085,7 +5087,7 @@
       <c r="E138" s="157"/>
       <c r="F138" s="158"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="48" t="s">
         <v>149</v>
       </c>
@@ -5097,7 +5099,7 @@
       <c r="E139" s="154"/>
       <c r="F139" s="155"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="48" t="s">
         <v>9</v>
       </c>
@@ -5109,7 +5111,7 @@
       <c r="E140" s="154"/>
       <c r="F140" s="155"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="48" t="s">
         <v>152</v>
       </c>
@@ -5121,7 +5123,7 @@
       <c r="E141" s="50"/>
       <c r="F141" s="51"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="48" t="s">
         <v>13</v>
       </c>
@@ -5131,7 +5133,7 @@
       <c r="E142" s="157"/>
       <c r="F142" s="158"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="48" t="s">
         <v>15</v>
       </c>
@@ -5151,7 +5153,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="53">
         <v>1</v>
       </c>
@@ -5165,7 +5167,7 @@
       <c r="E144" s="51"/>
       <c r="F144" s="55"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="53">
         <v>2</v>
       </c>
@@ -5181,7 +5183,7 @@
       <c r="E145" s="55"/>
       <c r="F145" s="55"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="53">
         <v>3</v>
       </c>
@@ -5195,7 +5197,7 @@
       <c r="E146" s="55"/>
       <c r="F146" s="55"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="53">
         <v>4</v>
       </c>
@@ -5209,7 +5211,7 @@
       <c r="E147" s="51"/>
       <c r="F147" s="55"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="53">
         <v>4</v>
       </c>
@@ -5223,7 +5225,7 @@
       <c r="E148" s="51"/>
       <c r="F148" s="55"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="53">
         <v>6</v>
       </c>
@@ -5237,7 +5239,7 @@
       <c r="E149" s="51"/>
       <c r="F149" s="55"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="53">
         <v>7</v>
       </c>
@@ -5251,7 +5253,7 @@
       <c r="E150" s="55"/>
       <c r="F150" s="55"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="53">
         <v>8</v>
       </c>
@@ -5265,7 +5267,7 @@
       <c r="E151" s="51"/>
       <c r="F151" s="55"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="53">
         <v>9</v>
       </c>
@@ -5279,7 +5281,7 @@
       <c r="E152" s="55"/>
       <c r="F152" s="55"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="53">
         <v>10</v>
       </c>
@@ -5345,7 +5347,7 @@
       <c r="E157" s="60"/>
       <c r="F157" s="60"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="47" t="s">
         <v>2</v>
       </c>
@@ -5357,7 +5359,7 @@
       <c r="E158" s="154"/>
       <c r="F158" s="155"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="48" t="s">
         <v>3</v>
       </c>
@@ -5369,7 +5371,7 @@
       <c r="E159" s="154"/>
       <c r="F159" s="155"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="48" t="s">
         <v>146</v>
       </c>
@@ -5381,7 +5383,7 @@
       <c r="E160" s="154"/>
       <c r="F160" s="155"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="48" t="s">
         <v>148</v>
       </c>
@@ -5391,7 +5393,7 @@
       <c r="E161" s="157"/>
       <c r="F161" s="158"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="48" t="s">
         <v>6</v>
       </c>
@@ -5401,7 +5403,7 @@
       <c r="E162" s="157"/>
       <c r="F162" s="158"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="48" t="s">
         <v>149</v>
       </c>
@@ -5413,7 +5415,7 @@
       <c r="E163" s="154"/>
       <c r="F163" s="155"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="48" t="s">
         <v>9</v>
       </c>
@@ -5423,7 +5425,7 @@
       <c r="E164" s="157"/>
       <c r="F164" s="158"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="48" t="s">
         <v>178</v>
       </c>
@@ -5435,7 +5437,7 @@
       <c r="E165" s="50"/>
       <c r="F165" s="51"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="48" t="s">
         <v>13</v>
       </c>
@@ -5445,7 +5447,7 @@
       <c r="E166" s="157"/>
       <c r="F166" s="158"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="48" t="s">
         <v>15</v>
       </c>
@@ -5465,7 +5467,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="67"/>
       <c r="B168" s="54" t="s">
         <v>179</v>
@@ -5477,7 +5479,7 @@
       <c r="E168" s="51"/>
       <c r="F168" s="55"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="67"/>
       <c r="B169" s="54" t="s">
         <v>181</v>
@@ -5491,7 +5493,7 @@
       <c r="E169" s="55"/>
       <c r="F169" s="55"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="67"/>
       <c r="B170" s="54" t="s">
         <v>182</v>
@@ -5503,7 +5505,7 @@
       <c r="E170" s="55"/>
       <c r="F170" s="55"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="67"/>
       <c r="B171" s="54" t="s">
         <v>157</v>
@@ -5515,7 +5517,7 @@
       <c r="E171" s="51"/>
       <c r="F171" s="55"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="67"/>
       <c r="B172" s="54" t="s">
         <v>158</v>
@@ -5527,7 +5529,7 @@
       <c r="E172" s="51"/>
       <c r="F172" s="55"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="67"/>
       <c r="B173" s="54" t="s">
         <v>160</v>
@@ -5539,7 +5541,7 @@
       <c r="E173" s="51"/>
       <c r="F173" s="55"/>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="67"/>
       <c r="B174" s="54" t="s">
         <v>183</v>
@@ -5551,7 +5553,7 @@
       <c r="E174" s="55"/>
       <c r="F174" s="55"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="67"/>
       <c r="B175" s="54" t="s">
         <v>185</v>
@@ -5563,7 +5565,7 @@
       <c r="E175" s="51"/>
       <c r="F175" s="55"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="67"/>
       <c r="B176" s="54" t="s">
         <v>187</v>
@@ -5577,7 +5579,7 @@
       <c r="E176" s="55"/>
       <c r="F176" s="55"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="67"/>
       <c r="B177" s="54" t="s">
         <v>190</v>
@@ -5589,7 +5591,7 @@
       <c r="E177" s="55"/>
       <c r="F177" s="55"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="67"/>
       <c r="B178" s="54" t="s">
         <v>192</v>
@@ -5603,7 +5605,7 @@
       <c r="E178" s="55"/>
       <c r="F178" s="55"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="67"/>
       <c r="B179" s="54" t="s">
         <v>170</v>
@@ -5615,7 +5617,7 @@
       <c r="E179" s="55"/>
       <c r="F179" s="55"/>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="67"/>
       <c r="B180" s="55"/>
       <c r="C180" s="55"/>
@@ -5623,7 +5625,7 @@
       <c r="E180" s="55"/>
       <c r="F180" s="55"/>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="48" t="s">
         <v>2</v>
       </c>
@@ -5635,7 +5637,7 @@
       <c r="E181" s="154"/>
       <c r="F181" s="155"/>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="48" t="s">
         <v>3</v>
       </c>
@@ -5647,7 +5649,7 @@
       <c r="E182" s="154"/>
       <c r="F182" s="155"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="48" t="s">
         <v>146</v>
       </c>
@@ -5659,7 +5661,7 @@
       <c r="E183" s="154"/>
       <c r="F183" s="155"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="48" t="s">
         <v>148</v>
       </c>
@@ -5669,7 +5671,7 @@
       <c r="E184" s="157"/>
       <c r="F184" s="158"/>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="48" t="s">
         <v>6</v>
       </c>
@@ -5679,7 +5681,7 @@
       <c r="E185" s="157"/>
       <c r="F185" s="158"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="48" t="s">
         <v>149</v>
       </c>
@@ -5691,7 +5693,7 @@
       <c r="E186" s="154"/>
       <c r="F186" s="155"/>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="48" t="s">
         <v>9</v>
       </c>
@@ -5703,7 +5705,7 @@
       <c r="E187" s="154"/>
       <c r="F187" s="155"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="48" t="s">
         <v>178</v>
       </c>
@@ -5715,7 +5717,7 @@
       <c r="E188" s="50"/>
       <c r="F188" s="51"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" s="48" t="s">
         <v>13</v>
       </c>
@@ -5725,7 +5727,7 @@
       <c r="E189" s="157"/>
       <c r="F189" s="158"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="48" t="s">
         <v>15</v>
       </c>
@@ -5745,7 +5747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="53">
         <v>1</v>
       </c>
@@ -5759,7 +5761,7 @@
       <c r="E191" s="51"/>
       <c r="F191" s="55"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="53">
         <v>2</v>
       </c>
@@ -5775,7 +5777,7 @@
       <c r="E192" s="55"/>
       <c r="F192" s="55"/>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="53">
         <v>3</v>
       </c>
@@ -5789,7 +5791,7 @@
       <c r="E193" s="55"/>
       <c r="F193" s="55"/>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" s="53">
         <v>4</v>
       </c>
@@ -5803,7 +5805,7 @@
       <c r="E194" s="51"/>
       <c r="F194" s="55"/>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="53">
         <v>5</v>
       </c>
@@ -5817,7 +5819,7 @@
       <c r="E195" s="51"/>
       <c r="F195" s="55"/>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="53">
         <v>6</v>
       </c>
@@ -5831,7 +5833,7 @@
       <c r="E196" s="51"/>
       <c r="F196" s="55"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A197" s="53">
         <v>7</v>
       </c>
@@ -5847,7 +5849,7 @@
       <c r="E197" s="55"/>
       <c r="F197" s="55"/>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="53">
         <v>8</v>
       </c>
@@ -5861,7 +5863,7 @@
       <c r="E198" s="51"/>
       <c r="F198" s="55"/>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="53">
         <v>9</v>
       </c>
@@ -5875,7 +5877,7 @@
       <c r="E199" s="55"/>
       <c r="F199" s="55"/>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" s="53">
         <v>10</v>
       </c>
@@ -5889,7 +5891,7 @@
       <c r="E200" s="55"/>
       <c r="F200" s="55"/>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" s="53">
         <v>11</v>
       </c>
@@ -5903,7 +5905,7 @@
       <c r="E201" s="55"/>
       <c r="F201" s="55"/>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A203" s="47" t="s">
         <v>2</v>
       </c>
@@ -5915,7 +5917,7 @@
       <c r="E203" s="154"/>
       <c r="F203" s="155"/>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A204" s="48" t="s">
         <v>3</v>
       </c>
@@ -5927,7 +5929,7 @@
       <c r="E204" s="154"/>
       <c r="F204" s="155"/>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A205" s="48" t="s">
         <v>146</v>
       </c>
@@ -5939,7 +5941,7 @@
       <c r="E205" s="154"/>
       <c r="F205" s="155"/>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A206" s="48" t="s">
         <v>148</v>
       </c>
@@ -5949,7 +5951,7 @@
       <c r="E206" s="157"/>
       <c r="F206" s="158"/>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A207" s="48" t="s">
         <v>6</v>
       </c>
@@ -5959,7 +5961,7 @@
       <c r="E207" s="157"/>
       <c r="F207" s="158"/>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A208" s="48" t="s">
         <v>149</v>
       </c>
@@ -5971,7 +5973,7 @@
       <c r="E208" s="154"/>
       <c r="F208" s="155"/>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A209" s="48" t="s">
         <v>9</v>
       </c>
@@ -5983,7 +5985,7 @@
       <c r="E209" s="154"/>
       <c r="F209" s="155"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A210" s="48" t="s">
         <v>178</v>
       </c>
@@ -5995,7 +5997,7 @@
       <c r="E210" s="50"/>
       <c r="F210" s="51"/>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A211" s="48" t="s">
         <v>13</v>
       </c>
@@ -6005,7 +6007,7 @@
       <c r="E211" s="157"/>
       <c r="F211" s="158"/>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A212" s="48" t="s">
         <v>15</v>
       </c>
@@ -6025,7 +6027,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A213" s="67"/>
       <c r="B213" s="54" t="s">
         <v>211</v>
@@ -6037,7 +6039,7 @@
       <c r="E213" s="51"/>
       <c r="F213" s="55"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A214" s="67"/>
       <c r="B214" s="54" t="s">
         <v>181</v>
@@ -6051,7 +6053,7 @@
       <c r="E214" s="55"/>
       <c r="F214" s="55"/>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A215" s="67"/>
       <c r="B215" s="54" t="s">
         <v>182</v>
@@ -6063,7 +6065,7 @@
       <c r="E215" s="55"/>
       <c r="F215" s="55"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A216" s="67"/>
       <c r="B216" s="54" t="s">
         <v>212</v>
@@ -6075,7 +6077,7 @@
       <c r="E216" s="51"/>
       <c r="F216" s="55"/>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A217" s="67"/>
       <c r="B217" s="54" t="s">
         <v>158</v>
@@ -6087,7 +6089,7 @@
       <c r="E217" s="51"/>
       <c r="F217" s="55"/>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A218" s="67"/>
       <c r="B218" s="54" t="s">
         <v>160</v>
@@ -6099,7 +6101,7 @@
       <c r="E218" s="51"/>
       <c r="F218" s="55"/>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A219" s="67"/>
       <c r="B219" s="54" t="s">
         <v>213</v>
@@ -6113,7 +6115,7 @@
       <c r="E219" s="55"/>
       <c r="F219" s="55"/>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A220" s="67"/>
       <c r="B220" s="54" t="s">
         <v>216</v>
@@ -6127,7 +6129,7 @@
       <c r="E220" s="51"/>
       <c r="F220" s="55"/>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A221" s="67"/>
       <c r="B221" s="54" t="s">
         <v>172</v>
@@ -6139,7 +6141,7 @@
       <c r="E221" s="55"/>
       <c r="F221" s="55"/>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A222" s="67"/>
       <c r="B222" s="54" t="s">
         <v>207</v>
@@ -6153,16 +6155,55 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
     <mergeCell ref="B209:F209"/>
     <mergeCell ref="B211:F211"/>
     <mergeCell ref="B185:F185"/>
@@ -6172,55 +6213,16 @@
     <mergeCell ref="B203:F203"/>
     <mergeCell ref="B204:F204"/>
     <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
@@ -6291,7 +6293,7 @@
       <c r="A2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="171" t="s">
         <v>221</v>
       </c>
       <c r="C2" s="154"/>
@@ -6319,7 +6321,7 @@
       <c r="A3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="172" t="s">
+      <c r="B3" s="171" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="154"/>
@@ -6347,7 +6349,7 @@
       <c r="A4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="171" t="s">
         <v>222</v>
       </c>
       <c r="C4" s="154"/>
@@ -6375,7 +6377,7 @@
       <c r="A5" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="172"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="154"/>
       <c r="D5" s="154"/>
       <c r="E5" s="154"/>
@@ -6401,7 +6403,7 @@
       <c r="A6" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="171" t="s">
         <v>223</v>
       </c>
       <c r="C6" s="154"/>
@@ -6429,7 +6431,7 @@
       <c r="A7" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="172" t="s">
+      <c r="B7" s="171" t="s">
         <v>224</v>
       </c>
       <c r="C7" s="154"/>
@@ -6457,7 +6459,7 @@
       <c r="A8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="172" t="s">
+      <c r="B8" s="171" t="s">
         <v>225</v>
       </c>
       <c r="C8" s="154"/>
@@ -7195,7 +7197,7 @@
       <c r="A32" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="172" t="s">
+      <c r="B32" s="171" t="s">
         <v>259</v>
       </c>
       <c r="C32" s="154"/>
@@ -7224,7 +7226,7 @@
       <c r="A33" s="81" t="s">
         <v>260</v>
       </c>
-      <c r="B33" s="172" t="s">
+      <c r="B33" s="171" t="s">
         <v>261</v>
       </c>
       <c r="C33" s="154"/>
@@ -7253,7 +7255,7 @@
       <c r="A34" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="172" t="s">
+      <c r="B34" s="171" t="s">
         <v>262</v>
       </c>
       <c r="C34" s="154"/>
@@ -7282,7 +7284,7 @@
       <c r="A35" s="81" t="s">
         <v>263</v>
       </c>
-      <c r="B35" s="172"/>
+      <c r="B35" s="171"/>
       <c r="C35" s="154"/>
       <c r="D35" s="154"/>
       <c r="E35" s="154"/>
@@ -7309,7 +7311,7 @@
       <c r="A36" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="B36" s="172" t="s">
+      <c r="B36" s="171" t="s">
         <v>264</v>
       </c>
       <c r="C36" s="154"/>
@@ -7338,7 +7340,7 @@
       <c r="A37" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="172" t="s">
+      <c r="B37" s="171" t="s">
         <v>224</v>
       </c>
       <c r="C37" s="154"/>
@@ -7367,7 +7369,7 @@
       <c r="A38" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="172" t="s">
+      <c r="B38" s="171" t="s">
         <v>225</v>
       </c>
       <c r="C38" s="154"/>
@@ -8236,7 +8238,7 @@
       <c r="A66" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="B66" s="171" t="s">
+      <c r="B66" s="172" t="s">
         <v>289</v>
       </c>
       <c r="C66" s="157"/>
@@ -8268,7 +8270,7 @@
       <c r="A67" s="89" t="s">
         <v>260</v>
       </c>
-      <c r="B67" s="171" t="s">
+      <c r="B67" s="172" t="s">
         <v>290</v>
       </c>
       <c r="C67" s="157"/>
@@ -8300,7 +8302,7 @@
       <c r="A68" s="89" t="s">
         <v>146</v>
       </c>
-      <c r="B68" s="171" t="s">
+      <c r="B68" s="172" t="s">
         <v>262</v>
       </c>
       <c r="C68" s="157"/>
@@ -8362,7 +8364,7 @@
       <c r="A70" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="B70" s="171" t="s">
+      <c r="B70" s="172" t="s">
         <v>264</v>
       </c>
       <c r="C70" s="157"/>
@@ -8394,7 +8396,7 @@
       <c r="A71" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B71" s="171" t="s">
+      <c r="B71" s="172" t="s">
         <v>224</v>
       </c>
       <c r="C71" s="157"/>
@@ -8426,7 +8428,7 @@
       <c r="A72" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B72" s="171" t="s">
+      <c r="B72" s="172" t="s">
         <v>225</v>
       </c>
       <c r="C72" s="157"/>
@@ -9851,16 +9853,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
     <mergeCell ref="B69:F69"/>
     <mergeCell ref="B70:F70"/>
     <mergeCell ref="B71:F71"/>
@@ -9872,6 +9864,16 @@
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
@@ -9934,7 +9936,7 @@
       <c r="A2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="172"/>
+      <c r="B2" s="171"/>
       <c r="C2" s="154"/>
       <c r="D2" s="154"/>
       <c r="E2" s="154"/>
@@ -9960,7 +9962,7 @@
       <c r="A3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="172" t="s">
+      <c r="B3" s="171" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="154"/>
@@ -9988,7 +9990,7 @@
       <c r="A4" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="172"/>
+      <c r="B4" s="171"/>
       <c r="C4" s="154"/>
       <c r="D4" s="154"/>
       <c r="E4" s="154"/>
@@ -10014,7 +10016,7 @@
       <c r="A5" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="172"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="154"/>
       <c r="D5" s="154"/>
       <c r="E5" s="154"/>
@@ -10040,7 +10042,7 @@
       <c r="A6" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="171" t="s">
         <v>303</v>
       </c>
       <c r="C6" s="154"/>
@@ -10068,7 +10070,7 @@
       <c r="A7" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="172" t="s">
+      <c r="B7" s="171" t="s">
         <v>304</v>
       </c>
       <c r="C7" s="154"/>
@@ -10124,7 +10126,7 @@
       <c r="A9" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="172"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="154"/>
       <c r="D9" s="154"/>
       <c r="E9" s="154"/>
@@ -10544,7 +10546,7 @@
       <c r="A23" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="176" t="s">
+      <c r="B23" s="173" t="s">
         <v>314</v>
       </c>
       <c r="C23" s="154"/>
@@ -10573,7 +10575,7 @@
       <c r="A24" s="81" t="s">
         <v>260</v>
       </c>
-      <c r="B24" s="176" t="s">
+      <c r="B24" s="173" t="s">
         <v>261</v>
       </c>
       <c r="C24" s="154"/>
@@ -10602,7 +10604,7 @@
       <c r="A25" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="172"/>
+      <c r="B25" s="171"/>
       <c r="C25" s="154"/>
       <c r="D25" s="154"/>
       <c r="E25" s="154"/>
@@ -10629,7 +10631,7 @@
       <c r="A26" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="172"/>
+      <c r="B26" s="171"/>
       <c r="C26" s="154"/>
       <c r="D26" s="154"/>
       <c r="E26" s="154"/>
@@ -10656,7 +10658,7 @@
       <c r="A27" s="81" t="s">
         <v>263</v>
       </c>
-      <c r="B27" s="172"/>
+      <c r="B27" s="171"/>
       <c r="C27" s="154"/>
       <c r="D27" s="154"/>
       <c r="E27" s="154"/>
@@ -10683,7 +10685,7 @@
       <c r="A28" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="B28" s="172"/>
+      <c r="B28" s="171"/>
       <c r="C28" s="154"/>
       <c r="D28" s="154"/>
       <c r="E28" s="154"/>
@@ -10760,7 +10762,7 @@
       <c r="A31" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="172"/>
+      <c r="B31" s="171"/>
       <c r="C31" s="154"/>
       <c r="D31" s="154"/>
       <c r="E31" s="154"/>
@@ -10787,7 +10789,7 @@
       <c r="A32" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="172"/>
+      <c r="B32" s="171"/>
       <c r="C32" s="154"/>
       <c r="D32" s="154"/>
       <c r="E32" s="154"/>
@@ -11101,7 +11103,7 @@
       <c r="A44" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="173"/>
+      <c r="B44" s="174"/>
       <c r="C44" s="155"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
@@ -11155,7 +11157,7 @@
       <c r="A46" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="174"/>
+      <c r="B46" s="176"/>
       <c r="C46" s="155"/>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
@@ -11236,7 +11238,7 @@
       <c r="A49" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="B49" s="174"/>
+      <c r="B49" s="176"/>
       <c r="C49" s="155"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
@@ -11263,7 +11265,7 @@
       <c r="A50" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="174"/>
+      <c r="B50" s="176"/>
       <c r="C50" s="155"/>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
@@ -11290,7 +11292,7 @@
       <c r="A51" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B51" s="174"/>
+      <c r="B51" s="176"/>
       <c r="C51" s="155"/>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
@@ -11529,7 +11531,7 @@
       <c r="A60" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="173" t="s">
+      <c r="B60" s="174" t="s">
         <v>315</v>
       </c>
       <c r="C60" s="154"/>
@@ -11558,7 +11560,7 @@
       <c r="A61" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="173"/>
+      <c r="B61" s="174"/>
       <c r="C61" s="154"/>
       <c r="D61" s="154"/>
       <c r="E61" s="154"/>
@@ -11585,7 +11587,7 @@
       <c r="A62" s="71" t="s">
         <v>316</v>
       </c>
-      <c r="B62" s="173"/>
+      <c r="B62" s="174"/>
       <c r="C62" s="154"/>
       <c r="D62" s="154"/>
       <c r="E62" s="154"/>
@@ -11612,7 +11614,7 @@
       <c r="A63" s="71" t="s">
         <v>148</v>
       </c>
-      <c r="B63" s="173"/>
+      <c r="B63" s="174"/>
       <c r="C63" s="154"/>
       <c r="D63" s="154"/>
       <c r="E63" s="154"/>
@@ -11639,7 +11641,7 @@
       <c r="A64" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="173"/>
+      <c r="B64" s="174"/>
       <c r="C64" s="154"/>
       <c r="D64" s="154"/>
       <c r="E64" s="154"/>
@@ -11666,7 +11668,7 @@
       <c r="A65" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="173"/>
+      <c r="B65" s="174"/>
       <c r="C65" s="154"/>
       <c r="D65" s="154"/>
       <c r="E65" s="154"/>
@@ -11693,7 +11695,7 @@
       <c r="A66" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B66" s="173"/>
+      <c r="B66" s="174"/>
       <c r="C66" s="154"/>
       <c r="D66" s="154"/>
       <c r="E66" s="154"/>
@@ -11720,7 +11722,7 @@
       <c r="A67" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B67" s="173"/>
+      <c r="B67" s="174"/>
       <c r="C67" s="154"/>
       <c r="D67" s="154"/>
       <c r="E67" s="154"/>
@@ -12009,7 +12011,7 @@
       <c r="A78" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="172"/>
+      <c r="B78" s="171"/>
       <c r="C78" s="154"/>
       <c r="D78" s="154"/>
       <c r="E78" s="154"/>
@@ -12036,7 +12038,7 @@
       <c r="A79" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B79" s="172"/>
+      <c r="B79" s="171"/>
       <c r="C79" s="154"/>
       <c r="D79" s="154"/>
       <c r="E79" s="154"/>
@@ -12063,7 +12065,7 @@
       <c r="A80" s="71" t="s">
         <v>318</v>
       </c>
-      <c r="B80" s="172"/>
+      <c r="B80" s="171"/>
       <c r="C80" s="154"/>
       <c r="D80" s="154"/>
       <c r="E80" s="154"/>
@@ -12090,7 +12092,7 @@
       <c r="A81" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="172"/>
+      <c r="B81" s="171"/>
       <c r="C81" s="154"/>
       <c r="D81" s="154"/>
       <c r="E81" s="154"/>
@@ -12117,7 +12119,7 @@
       <c r="A82" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="172"/>
+      <c r="B82" s="171"/>
       <c r="C82" s="154"/>
       <c r="D82" s="154"/>
       <c r="E82" s="154"/>
@@ -12144,7 +12146,7 @@
       <c r="A83" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="172"/>
+      <c r="B83" s="171"/>
       <c r="C83" s="154"/>
       <c r="D83" s="154"/>
       <c r="E83" s="154"/>
@@ -12171,7 +12173,7 @@
       <c r="A84" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B84" s="172"/>
+      <c r="B84" s="171"/>
       <c r="C84" s="154"/>
       <c r="D84" s="154"/>
       <c r="E84" s="154"/>
@@ -12510,7 +12512,7 @@
       <c r="A97" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B97" s="172"/>
+      <c r="B97" s="171"/>
       <c r="C97" s="154"/>
       <c r="D97" s="154"/>
       <c r="E97" s="154"/>
@@ -12537,7 +12539,7 @@
       <c r="A98" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B98" s="172"/>
+      <c r="B98" s="171"/>
       <c r="C98" s="154"/>
       <c r="D98" s="154"/>
       <c r="E98" s="154"/>
@@ -12564,7 +12566,7 @@
       <c r="A99" s="71" t="s">
         <v>319</v>
       </c>
-      <c r="B99" s="172"/>
+      <c r="B99" s="171"/>
       <c r="C99" s="154"/>
       <c r="D99" s="154"/>
       <c r="E99" s="154"/>
@@ -12591,7 +12593,7 @@
       <c r="A100" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="172"/>
+      <c r="B100" s="171"/>
       <c r="C100" s="154"/>
       <c r="D100" s="154"/>
       <c r="E100" s="154"/>
@@ -12618,7 +12620,7 @@
       <c r="A101" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="172"/>
+      <c r="B101" s="171"/>
       <c r="C101" s="154"/>
       <c r="D101" s="154"/>
       <c r="E101" s="154"/>
@@ -12645,7 +12647,7 @@
       <c r="A102" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="172"/>
+      <c r="B102" s="171"/>
       <c r="C102" s="154"/>
       <c r="D102" s="154"/>
       <c r="E102" s="154"/>
@@ -12672,7 +12674,7 @@
       <c r="A103" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B103" s="172"/>
+      <c r="B103" s="171"/>
       <c r="C103" s="154"/>
       <c r="D103" s="154"/>
       <c r="E103" s="154"/>
@@ -17980,41 +17982,6 @@
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
     <mergeCell ref="B101:F101"/>
     <mergeCell ref="B102:F102"/>
     <mergeCell ref="B103:F103"/>
@@ -18025,6 +17992,41 @@
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B99:F99"/>
     <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
@@ -18390,7 +18392,7 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>